<commit_message>
convert text columns to number in Excel
</commit_message>
<xml_diff>
--- a/inst/extdata/fluxes/lf_05/lf_05_b_2018-11-25.xlsx
+++ b/inst/extdata/fluxes/lf_05/lf_05_b_2018-11-25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Documents/data_working/data_packages/hypoxia.flux.analysis.1/inst/extdata/fluxes/lf_05/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Dropbox (Partners HealthCare)/Copeland.2021.hypoxia.flux/inst/extdata/fluxes/lf_05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F517346-F7E1-8E44-B47A-D879C71E3DD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE62428E-32EF-0349-B678-0F979577C930}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19360" yWindow="2140" windowWidth="25600" windowHeight="15540" xr2:uid="{1D4C4C2F-7A99-D141-A4DB-2424DC3A3300}"/>
+    <workbookView xWindow="9420" yWindow="2540" windowWidth="25600" windowHeight="15540" activeTab="5" xr2:uid="{1D4C4C2F-7A99-D141-A4DB-2424DC3A3300}"/>
   </bookViews>
   <sheets>
     <sheet name="evap" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -208,27 +208,6 @@
     <t>run</t>
   </si>
   <si>
-    <t>89.264</t>
-  </si>
-  <si>
-    <t>88.293</t>
-  </si>
-  <si>
-    <t>81.775</t>
-  </si>
-  <si>
-    <t>81.958</t>
-  </si>
-  <si>
-    <t>74.027</t>
-  </si>
-  <si>
-    <t>6.948</t>
-  </si>
-  <si>
-    <t>2330.111</t>
-  </si>
-  <si>
     <t>oxygen</t>
   </si>
   <si>
@@ -239,7 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -268,10 +247,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -590,15 +573,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0473DBDA-133C-8E46-809A-4027CD08C62D}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>
@@ -610,12 +593,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C2">
         <v>-24</v>
@@ -624,12 +607,12 @@
         <v>40.532800000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -638,12 +621,12 @@
         <v>52.226399999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>24</v>
@@ -652,12 +635,12 @@
         <v>51.8551</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C5">
         <v>48</v>
@@ -666,12 +649,12 @@
         <v>51.526800000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <v>72</v>
@@ -680,12 +663,12 @@
         <v>51.205300000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C7">
         <v>96</v>
@@ -694,12 +677,12 @@
         <v>50.911000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C8">
         <v>-24</v>
@@ -708,12 +691,12 @@
         <v>39.692900000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -722,12 +705,12 @@
         <v>51.446199999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C10">
         <v>24</v>
@@ -736,12 +719,12 @@
         <v>51.041600000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C11">
         <v>48</v>
@@ -750,12 +733,12 @@
         <v>50.859400000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C12">
         <v>72</v>
@@ -764,12 +747,12 @@
         <v>50.636299999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C13">
         <v>96</v>
@@ -791,9 +774,9 @@
       <selection activeCell="A2" sqref="A2:A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -813,7 +796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -824,7 +807,7 @@
         <v>118420</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -836,7 +819,7 @@
         <v>3404316</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -848,7 +831,7 @@
         <v>7104383</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -860,7 +843,7 @@
         <v>12202480</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -872,7 +855,7 @@
         <v>23489448</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -883,7 +866,7 @@
         <v>47737244</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -900,7 +883,7 @@
         <v>3669345</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -918,7 +901,7 @@
         <v>3550820</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -936,7 +919,7 @@
         <v>2132722</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -954,7 +937,7 @@
         <v>7995302</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -972,7 +955,7 @@
         <v>8668434</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -990,7 +973,7 @@
         <v>7105944</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1008,7 +991,7 @@
         <v>11485777</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1026,7 +1009,7 @@
         <v>15070672</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1044,7 +1027,7 @@
         <v>13375306</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1062,7 +1045,7 @@
         <v>17435998</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1080,7 +1063,7 @@
         <v>13688998</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1098,7 +1081,7 @@
         <v>15471420</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1116,7 +1099,7 @@
         <v>15024904</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1134,7 +1117,7 @@
         <v>16355395</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1152,7 +1135,7 @@
         <v>23168026</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1170,7 +1153,7 @@
         <v>2603924</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1188,7 +1171,7 @@
         <v>2410631</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1206,7 +1189,7 @@
         <v>3147002</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1224,7 +1207,7 @@
         <v>2914636</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1242,7 +1225,7 @@
         <v>4965458</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1260,7 +1243,7 @@
         <v>4304624</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1278,7 +1261,7 @@
         <v>4163726</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1296,7 +1279,7 @@
         <v>5854846</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1314,7 +1297,7 @@
         <v>4833470</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1332,7 +1315,7 @@
         <v>6309448</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1350,7 +1333,7 @@
         <v>5500753</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1368,7 +1351,7 @@
         <v>9329476</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1386,7 +1369,7 @@
         <v>9383469</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1404,7 +1387,7 @@
         <v>9678333</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1435,9 +1418,9 @@
       <selection activeCell="A2" sqref="A2:A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1451,7 +1434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1462,7 +1445,7 @@
         <v>3.5499999999999997E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1473,7 +1456,7 @@
         <v>0.14960000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1484,7 +1467,7 @@
         <v>0.28910000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1495,7 +1478,7 @@
         <v>0.433</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1506,7 +1489,7 @@
         <v>0.61580000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1517,7 +1500,7 @@
         <v>0.872</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1528,7 +1511,7 @@
         <v>1.1391</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1539,7 +1522,7 @@
         <v>1.3975</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1550,7 +1533,7 @@
         <v>0.8044</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1562,7 +1545,7 @@
         <v>0.79579999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1574,7 +1557,7 @@
         <v>0.8054</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1586,7 +1569,7 @@
         <v>0.84899999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1598,7 +1581,7 @@
         <v>0.79779999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1610,7 +1593,7 @@
         <v>0.80249999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1622,7 +1605,7 @@
         <v>0.73839999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1634,7 +1617,7 @@
         <v>0.75580000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1646,7 +1629,7 @@
         <v>0.7641</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1658,7 +1641,7 @@
         <v>0.72250000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1670,7 +1653,7 @@
         <v>0.69910000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1682,7 +1665,7 @@
         <v>0.70409999999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1694,7 +1677,7 @@
         <v>0.64649999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1706,7 +1689,7 @@
         <v>0.62680000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1718,7 +1701,7 @@
         <v>0.66390000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1730,7 +1713,7 @@
         <v>0.78669999999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1742,7 +1725,7 @@
         <v>0.80989999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1754,7 +1737,7 @@
         <v>0.83760000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1766,7 +1749,7 @@
         <v>0.79990000000000006</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1778,7 +1761,7 @@
         <v>0.79749999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1790,7 +1773,7 @@
         <v>0.8347</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1802,7 +1785,7 @@
         <v>0.7974</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1814,7 +1797,7 @@
         <v>0.76470000000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1826,7 +1809,7 @@
         <v>0.80569999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1838,7 +1821,7 @@
         <v>0.78559999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1850,7 +1833,7 @@
         <v>0.73629999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1862,7 +1845,7 @@
         <v>0.79369999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1874,7 +1857,7 @@
         <v>0.77229999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1886,7 +1869,7 @@
         <v>0.72740000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1911,9 +1894,9 @@
       <selection activeCell="A2" sqref="A2:A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1927,7 +1910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1938,7 +1921,7 @@
         <v>99033840</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1949,7 +1932,7 @@
         <v>137485808</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1960,7 +1943,7 @@
         <v>184429088</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1971,7 +1954,7 @@
         <v>282524608</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1982,7 +1965,7 @@
         <v>539872128</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1993,7 +1976,7 @@
         <v>1050655488</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2004,7 +1987,7 @@
         <v>1605349504</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2015,7 +1998,7 @@
         <v>2521874944</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2026,7 +2009,7 @@
         <v>101498328</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2038,7 +2021,7 @@
         <v>106162192</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2050,7 +2033,7 @@
         <v>106582456</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2062,7 +2045,7 @@
         <v>212946112</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2074,7 +2057,7 @@
         <v>203505184</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2086,7 +2069,7 @@
         <v>220948928</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2098,7 +2081,7 @@
         <v>408825984</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2110,7 +2093,7 @@
         <v>372859584</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2122,7 +2105,7 @@
         <v>383619328</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2134,7 +2117,7 @@
         <v>736911744</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2146,7 +2129,7 @@
         <v>731407744</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2158,7 +2141,7 @@
         <v>723420032</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2170,7 +2153,7 @@
         <v>1199399424</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2182,7 +2165,7 @@
         <v>1110571520</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -2194,7 +2177,7 @@
         <v>1171769728</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2206,7 +2189,7 @@
         <v>110040136</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -2218,7 +2201,7 @@
         <v>103722880</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -2230,7 +2213,7 @@
         <v>107333944</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -2242,7 +2225,7 @@
         <v>151082224</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -2254,7 +2237,7 @@
         <v>154179680</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -2266,7 +2249,7 @@
         <v>149444176</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -2278,7 +2261,7 @@
         <v>242522784</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2290,7 +2273,7 @@
         <v>232430384</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2302,7 +2285,7 @@
         <v>213021840</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -2314,7 +2297,7 @@
         <v>327018208</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2326,7 +2309,7 @@
         <v>325823232</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -2338,7 +2321,7 @@
         <v>343130944</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -2350,7 +2333,7 @@
         <v>655609472</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -2362,7 +2345,7 @@
         <v>505430048</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -2387,9 +2370,9 @@
       <selection activeCell="A2" sqref="A2:A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -2403,7 +2386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2414,7 +2397,7 @@
         <v>53464608</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2425,7 +2408,7 @@
         <v>66304088</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2436,7 +2419,7 @@
         <v>83823352</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2447,7 +2430,7 @@
         <v>137101312</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2458,7 +2441,7 @@
         <v>237194816</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2469,7 +2452,7 @@
         <v>357991232</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2480,7 +2463,7 @@
         <v>472840512</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2491,7 +2474,7 @@
         <v>572865152</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2502,7 +2485,7 @@
         <v>309818016</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2514,7 +2497,7 @@
         <v>325849184</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2526,7 +2509,7 @@
         <v>335816384</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2538,7 +2521,7 @@
         <v>335559616</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2550,7 +2533,7 @@
         <v>329193184</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2562,7 +2545,7 @@
         <v>320231232</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2574,7 +2557,7 @@
         <v>315838400</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2586,7 +2569,7 @@
         <v>281128032</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2598,7 +2581,7 @@
         <v>290203648</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2610,7 +2593,7 @@
         <v>273240032</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2622,7 +2605,7 @@
         <v>258510336</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2634,7 +2617,7 @@
         <v>252824112</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2645,7 +2628,7 @@
         <v>325186688</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2657,7 +2640,7 @@
         <v>340555232</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -2669,7 +2652,7 @@
         <v>326612160</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2681,7 +2664,7 @@
         <v>318694528</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -2693,7 +2676,7 @@
         <v>324737184</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -2705,7 +2688,7 @@
         <v>315771136</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -2717,7 +2700,7 @@
         <v>322525088</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -2729,7 +2712,7 @@
         <v>319399808</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -2741,7 +2724,7 @@
         <v>325694208</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -2753,7 +2736,7 @@
         <v>300612800</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2765,7 +2748,7 @@
         <v>294026880</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2777,7 +2760,7 @@
         <v>313104352</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -2788,7 +2771,7 @@
         <v>333648320</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2800,7 +2783,7 @@
         <v>328757664</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -2812,7 +2795,7 @@
         <v>316224896</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -2824,7 +2807,7 @@
         <v>332814016</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -2836,7 +2819,7 @@
         <v>338912832</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -2848,7 +2831,7 @@
         <v>340748064</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -2860,7 +2843,7 @@
         <v>357026976</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -2872,7 +2855,7 @@
         <v>338168864</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -2884,7 +2867,7 @@
         <v>355507840</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -2896,7 +2879,7 @@
         <v>377122048</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -2908,7 +2891,7 @@
         <v>346390816</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -2920,7 +2903,7 @@
         <v>362689568</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -2931,7 +2914,7 @@
         <v>322417984</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -2943,7 +2926,7 @@
         <v>320585280</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -2955,7 +2938,7 @@
         <v>334415616</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -2967,7 +2950,7 @@
         <v>359268576</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -2979,7 +2962,7 @@
         <v>333024896</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -2991,7 +2974,7 @@
         <v>332880640</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -3003,7 +2986,7 @@
         <v>364256768</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -3015,7 +2998,7 @@
         <v>341656768</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -3036,16 +3019,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB109D08-A5B1-6D4B-A447-26B54BD3B22D}">
   <dimension ref="A1:AV63"/>
   <sheetViews>
-    <sheetView topLeftCell="AD34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AI41" workbookViewId="0">
       <selection activeCell="AK63" sqref="AK63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="31" max="31" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -3191,7 +3174,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:48">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3331,7 +3314,7 @@
         <v>35.460099999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:48">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3471,7 +3454,7 @@
         <v>85.93</v>
       </c>
     </row>
-    <row r="4" spans="1:48">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3614,7 +3597,7 @@
         <v>370.03120000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:48">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3757,7 +3740,7 @@
         <v>935.01969999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:48">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3900,7 +3883,7 @@
         <v>2419.8371999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:48">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4040,7 +4023,7 @@
         <v>2036.8662999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:48">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -4177,7 +4160,7 @@
         <v>1837.5771</v>
       </c>
     </row>
-    <row r="9" spans="1:48">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -4317,7 +4300,7 @@
         <v>2225.7136</v>
       </c>
     </row>
-    <row r="10" spans="1:48">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -4457,7 +4440,7 @@
         <v>2131.3215</v>
       </c>
     </row>
-    <row r="11" spans="1:48">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -4594,7 +4577,7 @@
         <v>1661.9401</v>
       </c>
     </row>
-    <row r="12" spans="1:48">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -4731,7 +4714,7 @@
         <v>1841.0592999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:48">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -4871,7 +4854,7 @@
         <v>2222.7831999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:48">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -5011,7 +4994,7 @@
         <v>2095.2366000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:48">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -5151,7 +5134,7 @@
         <v>2286.3762000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:48">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -5291,7 +5274,7 @@
         <v>1893.1532</v>
       </c>
     </row>
-    <row r="17" spans="1:48">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -5428,7 +5411,7 @@
         <v>1677.2329</v>
       </c>
     </row>
-    <row r="18" spans="1:48">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -5565,7 +5548,7 @@
         <v>1780.9417000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:48">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -5705,7 +5688,7 @@
         <v>1777.5918999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:48">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -5845,7 +5828,7 @@
         <v>1949.1061</v>
       </c>
     </row>
-    <row r="21" spans="1:48">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -5985,7 +5968,7 @@
         <v>2185.3308000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:48">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -6125,7 +6108,7 @@
         <v>2180.1797000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:48">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -6265,7 +6248,7 @@
         <v>2150.0050999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:48">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -6402,7 +6385,7 @@
         <v>2027.5708</v>
       </c>
     </row>
-    <row r="25" spans="1:48">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -6542,7 +6525,7 @@
         <v>2150.6934000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:48">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -6679,7 +6662,7 @@
         <v>1930.8503000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:48">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -6819,7 +6802,7 @@
         <v>2092.7561000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:48">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -6959,7 +6942,7 @@
         <v>2274.5410000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:48">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -7099,7 +7082,7 @@
         <v>2134.3923</v>
       </c>
     </row>
-    <row r="30" spans="1:48">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -7239,7 +7222,7 @@
         <v>2232.7029000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:48">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -7376,7 +7359,7 @@
         <v>1867.1914999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:48">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -7516,7 +7499,7 @@
         <v>2154.0329999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:48">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -7653,7 +7636,7 @@
         <v>2040.1501000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:48">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -7793,7 +7776,7 @@
         <v>2196.6277</v>
       </c>
     </row>
-    <row r="35" spans="1:48">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -7933,7 +7916,7 @@
         <v>1864.4315999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:48">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -8073,7 +8056,7 @@
         <v>2308.0756999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:48">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -8213,7 +8196,7 @@
         <v>2259.8454999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:48">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -8353,7 +8336,7 @@
         <v>2231.2954</v>
       </c>
     </row>
-    <row r="39" spans="1:48">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -8493,7 +8476,7 @@
         <v>2215.7741999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:48">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -8633,7 +8616,7 @@
         <v>2246.4596999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:48">
+    <row r="41" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -8773,7 +8756,7 @@
         <v>2243.9919</v>
       </c>
     </row>
-    <row r="42" spans="1:48">
+    <row r="42" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -8858,8 +8841,8 @@
       <c r="AD42">
         <v>231.29259999999999</v>
       </c>
-      <c r="AE42" s="2" t="s">
-        <v>56</v>
+      <c r="AE42" s="4">
+        <v>89.263999999999996</v>
       </c>
       <c r="AF42">
         <v>2008.8634999999999</v>
@@ -8913,7 +8896,7 @@
         <v>2328.3971999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:48">
+    <row r="43" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -8935,8 +8918,8 @@
       <c r="H43">
         <v>14.3306</v>
       </c>
-      <c r="I43" t="s">
-        <v>61</v>
+      <c r="I43" s="3">
+        <v>6.9480000000000004</v>
       </c>
       <c r="J43">
         <v>285.70819999999998</v>
@@ -8998,8 +8981,8 @@
       <c r="AD43">
         <v>222.48580000000001</v>
       </c>
-      <c r="AE43" s="2" t="s">
-        <v>57</v>
+      <c r="AE43" s="4">
+        <v>88.293000000000006</v>
       </c>
       <c r="AF43">
         <v>1983.1498999999999</v>
@@ -9053,7 +9036,7 @@
         <v>2338.6718999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:48">
+    <row r="44" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -9138,8 +9121,8 @@
       <c r="AD44">
         <v>209.4308</v>
       </c>
-      <c r="AE44" s="2" t="s">
-        <v>58</v>
+      <c r="AE44" s="4">
+        <v>81.775000000000006</v>
       </c>
       <c r="AF44">
         <v>1925.0393999999999</v>
@@ -9193,7 +9176,7 @@
         <v>2263.2537000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:48">
+    <row r="45" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -9278,8 +9261,8 @@
       <c r="AD45">
         <v>209.19970000000001</v>
       </c>
-      <c r="AE45" s="2" t="s">
-        <v>59</v>
+      <c r="AE45" s="4">
+        <v>81.957999999999998</v>
       </c>
       <c r="AF45">
         <v>1922.8710000000001</v>
@@ -9330,7 +9313,7 @@
         <v>2250.5949999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:48">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -9415,8 +9398,8 @@
       <c r="AD46">
         <v>186.80799999999999</v>
       </c>
-      <c r="AE46" s="2" t="s">
-        <v>60</v>
+      <c r="AE46" s="4">
+        <v>74.027000000000001</v>
       </c>
       <c r="AF46">
         <v>1818.8668</v>
@@ -9467,7 +9450,7 @@
         <v>2142.2141000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:48">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -9604,7 +9587,7 @@
         <v>1848.8961999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:48">
+    <row r="48" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -9741,7 +9724,7 @@
         <v>2299.6718999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:48">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -9878,7 +9861,7 @@
         <v>2214.0270999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:48">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -10015,7 +9998,7 @@
         <v>2201.8717999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:48">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -10152,7 +10135,7 @@
         <v>2043.4717000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:48">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -10289,7 +10272,7 @@
         <v>2144.9375</v>
       </c>
     </row>
-    <row r="53" spans="1:48">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -10426,7 +10409,7 @@
         <v>1869.6801</v>
       </c>
     </row>
-    <row r="54" spans="1:48">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -10563,7 +10546,7 @@
         <v>2226.6745999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:48">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -10700,7 +10683,7 @@
         <v>1940.9203</v>
       </c>
     </row>
-    <row r="56" spans="1:48">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -10837,7 +10820,7 @@
         <v>1941.2090000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:48">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -10977,7 +10960,7 @@
         <v>2118.2660999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:48">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -11114,7 +11097,7 @@
         <v>2179.9281999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:48">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -11254,7 +11237,7 @@
         <v>2027.5172</v>
       </c>
     </row>
-    <row r="60" spans="1:48">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -11391,7 +11374,7 @@
         <v>1826.5126</v>
       </c>
     </row>
-    <row r="61" spans="1:48">
+    <row r="61" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -11528,7 +11511,7 @@
         <v>1981.2617</v>
       </c>
     </row>
-    <row r="62" spans="1:48">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -11668,7 +11651,7 @@
         <v>2284.7285000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:48">
+    <row r="63" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -11768,8 +11751,8 @@
       <c r="AJ63">
         <v>1578.6495</v>
       </c>
-      <c r="AK63" t="s">
-        <v>62</v>
+      <c r="AK63" s="3">
+        <v>2330.1109999999999</v>
       </c>
       <c r="AL63">
         <v>997.54859999999996</v>

</xml_diff>